<commit_message>
Updated test scripts with new loading details methods for Voltage Drop calculation and 5V
</commit_message>
<xml_diff>
--- a/Test Data/Verify Voltage Drop Calculation on adding devices in Multiple loops of FIM.xlsx
+++ b/Test Data/Verify Voltage Drop Calculation on adding devices in Multiple loops of FIM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jdhakaa\Documents\NG Consys Project\Testing\NGConsys Automation\Test Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A852A6E7-ADB0-473D-8E1C-3D545242F53A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5EC6223-DCC5-422B-AF19-E39F7FB4E4B2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19008" windowHeight="9024" xr2:uid="{909A8366-666E-4CCA-9776-5FB1A83C0292}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" activeTab="1" xr2:uid="{909A8366-666E-4CCA-9776-5FB1A83C0292}"/>
   </bookViews>
   <sheets>
     <sheet name="Add Devices Loop A" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="31">
   <si>
     <t xml:space="preserve">Note: Do not change the column/rows index </t>
   </si>
@@ -113,6 +113,18 @@
   </si>
   <si>
     <t>verifyVoltageDropCalculation</t>
+  </si>
+  <si>
+    <t>Volt Drop (V)</t>
+  </si>
+  <si>
+    <t>Volt Drop (worst case)</t>
+  </si>
+  <si>
+    <t>Volt drop loading detail name</t>
+  </si>
+  <si>
+    <t>Volt drop worst case loading detail name</t>
   </si>
 </sst>
 </file>
@@ -209,7 +221,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -218,10 +230,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -240,6 +248,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -557,8 +568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37698239-2F64-411E-8891-9071AB24FC45}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H5" sqref="H5:I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -574,93 +585,103 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="G1" s="20" t="s">
+      <c r="C1" s="11"/>
+      <c r="G1" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="20"/>
+      <c r="H1" s="18"/>
       <c r="I1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="13"/>
+      <c r="C2" s="11"/>
       <c r="G2" s="2"/>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="7" t="s">
         <v>18</v>
       </c>
       <c r="I2" s="4"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="11" t="s">
+    <row r="3" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="6" t="s">
         <v>16</v>
       </c>
+      <c r="E3" s="19" t="s">
+        <v>27</v>
+      </c>
       <c r="G3" s="5"/>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="7" t="s">
         <v>19</v>
       </c>
       <c r="I3" s="4"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="14"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="14" t="s">
+    <row r="4" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="12"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="10"/>
-      <c r="H4" s="9" t="s">
+      <c r="E4" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="8"/>
+      <c r="H4" s="7" t="s">
         <v>20</v>
       </c>
       <c r="I4" s="4"/>
     </row>
     <row r="5" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="17" t="s">
+      <c r="G5" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="6"/>
-      <c r="I5" s="7"/>
+      <c r="H5" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
@@ -675,14 +696,20 @@
       <c r="D6" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="8">
         <v>287</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="8">
         <v>0.46</v>
       </c>
-      <c r="G6" s="10">
+      <c r="G6" s="8">
         <v>0.86</v>
+      </c>
+      <c r="H6" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="I6" s="19" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -706,6 +733,12 @@
       </c>
       <c r="G7" s="1">
         <v>1.02</v>
+      </c>
+      <c r="H7" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" s="19" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -721,8 +754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F314061-75BE-4623-93F7-3EBA86CADE07}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5:I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -738,90 +771,102 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="G1" s="20" t="s">
+      <c r="C1" s="11"/>
+      <c r="G1" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="20"/>
+      <c r="H1" s="18"/>
       <c r="I1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="13"/>
+      <c r="C2" s="11"/>
       <c r="G2" s="2"/>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="7" t="s">
         <v>18</v>
       </c>
       <c r="I2" s="4"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="11" t="s">
+    <row r="3" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="6" t="s">
         <v>16</v>
       </c>
+      <c r="E3" s="19" t="s">
+        <v>27</v>
+      </c>
       <c r="G3" s="5"/>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="7" t="s">
         <v>19</v>
       </c>
       <c r="I3" s="4"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="14"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="14" t="s">
+    <row r="4" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="12"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="10"/>
-      <c r="H4" s="9" t="s">
+      <c r="E4" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="8"/>
+      <c r="H4" s="7" t="s">
         <v>20</v>
       </c>
       <c r="I4" s="4"/>
     </row>
     <row r="5" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="17" t="s">
+      <c r="G5" s="15" t="s">
         <v>3</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -845,6 +890,12 @@
       </c>
       <c r="G6" s="1">
         <v>0.86</v>
+      </c>
+      <c r="H6" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="I6" s="19" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -852,5 +903,6 @@
     <mergeCell ref="G1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>